<commit_message>
Update daily and intraday volume tables for Bond and E-mini Futures
- Adjusted average daily volume and differences for 10yr Bond Futures in Table 1.
- Modified average daily volume and differences for E-mini Futures in Table 1 and Table 2.
- Updated observations count for E-mini Futures in Table 1 and Table 2.
- Revised average daily volume and differences for E-mini Futures in Table 3 (Post-ZLB, Pre-ZLB, ZLB).
- Corrected observations count for E-mini Futures in Table 3.
- Ensured consistency across all related LaTeX and Excel files.
</commit_message>
<xml_diff>
--- a/output/table1/Table1_daily_volume_total.xlsx
+++ b/output/table1/Table1_daily_volume_total.xlsx
@@ -620,7 +620,7 @@
         <v>2660.22026431718</v>
       </c>
       <c r="E2" t="n">
-        <v>6953.776198605727</v>
+        <v>6953.776198605728</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -2385,40 +2385,40 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>902875.0181818182</v>
+        <v>898789.6108597285</v>
       </c>
       <c r="E26" t="n">
-        <v>864437.4727958788</v>
+        <v>864606.3589447475</v>
       </c>
       <c r="F26" t="n">
-        <v>2847.5</v>
+        <v>2468</v>
       </c>
       <c r="G26" t="n">
-        <v>1003486.5</v>
+        <v>1002885</v>
       </c>
       <c r="H26" t="n">
-        <v>1412161.5</v>
+        <v>1406731</v>
       </c>
       <c r="I26" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J26" t="n">
-        <v>1162865.027272727</v>
+        <v>1157603.194570136</v>
       </c>
       <c r="K26" t="n">
-        <v>955041.4966405799</v>
+        <v>956073.8115222843</v>
       </c>
       <c r="L26" t="n">
-        <v>496151.5</v>
+        <v>489073</v>
       </c>
       <c r="M26" t="n">
-        <v>1178702</v>
+        <v>1178049</v>
       </c>
       <c r="N26" t="n">
-        <v>1614857.75</v>
+        <v>1614520</v>
       </c>
       <c r="O26" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="P26" t="n">
         <v>1329454.090497738</v>
@@ -2439,40 +2439,40 @@
         <v>221</v>
       </c>
       <c r="V26" t="n">
-        <v>1406878.268181818</v>
+        <v>1400512.303167421</v>
       </c>
       <c r="W26" t="n">
-        <v>1051917.852346188</v>
+        <v>1053782.529173701</v>
       </c>
       <c r="X26" t="n">
-        <v>570873.5</v>
+        <v>568235</v>
       </c>
       <c r="Y26" t="n">
-        <v>1569477</v>
+        <v>1553653</v>
       </c>
       <c r="Z26" t="n">
-        <v>1984814.75</v>
+        <v>1984535</v>
       </c>
       <c r="AA26" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="AB26" t="n">
-        <v>1328034.208530806</v>
+        <v>1267942.162895928</v>
       </c>
       <c r="AC26" t="n">
-        <v>1020603.21336921</v>
+        <v>1034806.083474207</v>
       </c>
       <c r="AD26" t="n">
-        <v>602434</v>
+        <v>0</v>
       </c>
       <c r="AE26" t="n">
-        <v>1357062</v>
+        <v>1324144</v>
       </c>
       <c r="AF26" t="n">
-        <v>1967134.5</v>
+        <v>1916380</v>
       </c>
       <c r="AG26" t="n">
-        <v>211</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27">
@@ -2492,7 +2492,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>432622.0454545455</v>
+        <v>430664.479638009</v>
       </c>
       <c r="E27" t="inlineStr"/>
       <c r="F27" t="inlineStr"/>
@@ -2500,7 +2500,7 @@
       <c r="H27" t="inlineStr"/>
       <c r="I27" t="inlineStr"/>
       <c r="J27" t="n">
-        <v>172367.7136363636</v>
+        <v>171850.8959276018</v>
       </c>
       <c r="K27" t="inlineStr"/>
       <c r="L27" t="inlineStr"/>
@@ -2516,7 +2516,7 @@
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="n">
-        <v>-86124.98636363636</v>
+        <v>-71058.21266968326</v>
       </c>
       <c r="W27" t="inlineStr"/>
       <c r="X27" t="inlineStr"/>
@@ -2524,7 +2524,7 @@
       <c r="Z27" t="inlineStr"/>
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="n">
-        <v>5583.270142180095</v>
+        <v>61511.92760180996</v>
       </c>
       <c r="AC27" t="inlineStr"/>
       <c r="AD27" t="inlineStr"/>
@@ -2549,7 +2549,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E28" t="inlineStr"/>
       <c r="F28" t="inlineStr"/>
@@ -2557,7 +2557,7 @@
       <c r="H28" t="inlineStr"/>
       <c r="I28" t="inlineStr"/>
       <c r="J28" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="K28" t="inlineStr"/>
       <c r="L28" t="inlineStr"/>
@@ -2573,7 +2573,7 @@
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="n">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
@@ -2581,7 +2581,7 @@
       <c r="Z28" t="inlineStr"/>
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="n">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="AC28" t="inlineStr"/>
       <c r="AD28" t="inlineStr"/>

</xml_diff>

<commit_message>
Update volume tables with revised statistics and values for daily and intraday volumes around FOMC events. Adjusted data for Bond Futures and E-mini Futures across multiple tables, including changes in means, standard deviations, and number of observations. Updated LaTeX and Excel files to reflect the latest calculations and ensure consistency across outputs.
</commit_message>
<xml_diff>
--- a/output/table1/Table1_daily_volume_total.xlsx
+++ b/output/table1/Table1_daily_volume_total.xlsx
@@ -617,10 +617,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>2660.22026431718</v>
+        <v>2649.026431718062</v>
       </c>
       <c r="E2" t="n">
-        <v>6953.776198605728</v>
+        <v>6938.179297474234</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -635,10 +635,10 @@
         <v>227</v>
       </c>
       <c r="J2" t="n">
-        <v>4443.837004405286</v>
+        <v>4438.114537444934</v>
       </c>
       <c r="K2" t="n">
-        <v>12135.1528125133</v>
+        <v>12094.84137329755</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -653,10 +653,10 @@
         <v>227</v>
       </c>
       <c r="P2" t="n">
-        <v>11275.21145374449</v>
+        <v>11266.90748898678</v>
       </c>
       <c r="Q2" t="n">
-        <v>25894.54812113097</v>
+        <v>25891.47595910595</v>
       </c>
       <c r="R2" t="n">
         <v>0</v>
@@ -671,28 +671,28 @@
         <v>227</v>
       </c>
       <c r="V2" t="n">
-        <v>5664.321585903083</v>
+        <v>5669.88986784141</v>
       </c>
       <c r="W2" t="n">
-        <v>12142.47722198359</v>
+        <v>12141.26430089142</v>
       </c>
       <c r="X2" t="n">
         <v>0</v>
       </c>
       <c r="Y2" t="n">
-        <v>497</v>
+        <v>554</v>
       </c>
       <c r="Z2" t="n">
-        <v>5524</v>
+        <v>5524.5</v>
       </c>
       <c r="AA2" t="n">
         <v>227</v>
       </c>
       <c r="AB2" t="n">
-        <v>4440.925110132159</v>
+        <v>4443.290748898678</v>
       </c>
       <c r="AC2" t="n">
-        <v>10460.9000327107</v>
+        <v>10451.28341757045</v>
       </c>
       <c r="AD2" t="n">
         <v>0</v>
@@ -724,7 +724,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>8614.991189427314</v>
+        <v>8617.881057268722</v>
       </c>
       <c r="E3" t="inlineStr"/>
       <c r="F3" t="inlineStr"/>
@@ -732,7 +732,7 @@
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="n">
-        <v>6831.374449339207</v>
+        <v>6828.79295154185</v>
       </c>
       <c r="K3" t="inlineStr"/>
       <c r="L3" t="inlineStr"/>
@@ -748,7 +748,7 @@
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="n">
-        <v>5610.88986784141</v>
+        <v>5597.017621145375</v>
       </c>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
@@ -756,7 +756,7 @@
       <c r="Z3" t="inlineStr"/>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="n">
-        <v>6834.286343612334</v>
+        <v>6823.616740088106</v>
       </c>
       <c r="AC3" t="inlineStr"/>
       <c r="AD3" t="inlineStr"/>

</xml_diff>